<commit_message>
Customer and Invoice Detail download functionality added
</commit_message>
<xml_diff>
--- a/invoice_system_management/static/excel/invoice.xlsx
+++ b/invoice_system_management/static/excel/invoice.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +498,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B2" s="3" t="n">
@@ -520,26 +520,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>1002.21</v>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>bike</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>200</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
+        <v>1182.6078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>